<commit_message>
feature: updated xlsx data
</commit_message>
<xml_diff>
--- a/kart.xlsx
+++ b/kart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlos.moura/dev/kart-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6817B4F-648F-8046-850A-D28EC06A8B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE0079F-28DA-7D4B-BF04-0A2D66101D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="500" windowWidth="38400" windowHeight="19480" xr2:uid="{7E41A2EF-39A8-C44A-939A-3D747B152ADF}"/>
   </bookViews>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8E46D72-A74A-564D-9C1F-EB563349D53E}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>